<commit_message>
Pushing updates: Load level data into level manager at start.
</commit_message>
<xml_diff>
--- a/Design/Levels.xlsx
+++ b/Design/Levels.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Level Design</t>
   </si>
@@ -28673,7 +28673,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28690,10 +28690,10 @@
         <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>40</v>
@@ -28726,10 +28726,10 @@
         <v>20</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>46</v>
@@ -28749,10 +28749,10 @@
         <v>20</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>47</v>
@@ -28764,94 +28764,418 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" ht="60">
       <c r="A5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="60">
       <c r="A6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="60">
       <c r="A7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="60">
       <c r="A8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="60">
       <c r="A9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="60">
       <c r="A10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="60">
       <c r="A11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="60">
       <c r="A12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="B12">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="60">
       <c r="A13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="60">
       <c r="A14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="60">
       <c r="A15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="60">
       <c r="A16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60">
       <c r="A17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="60">
       <c r="A18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60">
       <c r="A19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60">
       <c r="A20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="60">
       <c r="A21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="60">
       <c r="A22">
         <v>20</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tweening to splash screen intro/outro
</commit_message>
<xml_diff>
--- a/Design/Levels.xlsx
+++ b/Design/Levels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Design Points" sheetId="1" r:id="rId1"/>
-    <sheet name="TASKS" sheetId="2" r:id="rId2"/>
+    <sheet name="_Design Points" sheetId="1" r:id="rId1"/>
+    <sheet name="_TASKS" sheetId="2" r:id="rId2"/>
     <sheet name="Levels" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -516,13 +516,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1"/>
@@ -28590,13 +28591,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="2" spans="2:3">
       <c r="B2" t="s">
@@ -28670,19 +28672,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="11.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="45">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="28.8">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
@@ -28718,7 +28721,7 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="3" spans="1:20" ht="60">
+    <row r="3" spans="1:20" ht="57.6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -28741,7 +28744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="60">
+    <row r="4" spans="1:20" ht="57.6">
       <c r="A4">
         <v>2</v>
       </c>
@@ -28764,7 +28767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="60">
+    <row r="5" spans="1:20" ht="57.6">
       <c r="A5">
         <v>3</v>
       </c>
@@ -28787,7 +28790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="60">
+    <row r="6" spans="1:20" ht="57.6">
       <c r="A6">
         <v>4</v>
       </c>
@@ -28810,7 +28813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="60">
+    <row r="7" spans="1:20" ht="57.6">
       <c r="A7">
         <v>5</v>
       </c>
@@ -28833,7 +28836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="60">
+    <row r="8" spans="1:20" ht="57.6">
       <c r="A8">
         <v>6</v>
       </c>
@@ -28856,7 +28859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="60">
+    <row r="9" spans="1:20" ht="57.6">
       <c r="A9">
         <v>7</v>
       </c>
@@ -28879,7 +28882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="60">
+    <row r="10" spans="1:20" ht="57.6">
       <c r="A10">
         <v>8</v>
       </c>
@@ -28902,7 +28905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="60">
+    <row r="11" spans="1:20" ht="57.6">
       <c r="A11">
         <v>9</v>
       </c>
@@ -28925,7 +28928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="60">
+    <row r="12" spans="1:20" ht="57.6">
       <c r="A12">
         <v>10</v>
       </c>
@@ -28948,7 +28951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="60">
+    <row r="13" spans="1:20" ht="57.6">
       <c r="A13">
         <v>11</v>
       </c>
@@ -28971,7 +28974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="60">
+    <row r="14" spans="1:20" ht="57.6">
       <c r="A14">
         <v>12</v>
       </c>
@@ -28994,7 +28997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="60">
+    <row r="15" spans="1:20" ht="57.6">
       <c r="A15">
         <v>13</v>
       </c>
@@ -29017,7 +29020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="60">
+    <row r="16" spans="1:20" ht="57.6">
       <c r="A16">
         <v>14</v>
       </c>
@@ -29040,7 +29043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60">
+    <row r="17" spans="1:7" ht="57.6">
       <c r="A17">
         <v>15</v>
       </c>
@@ -29063,7 +29066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="60">
+    <row r="18" spans="1:7" ht="57.6">
       <c r="A18">
         <v>16</v>
       </c>
@@ -29086,7 +29089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="60">
+    <row r="19" spans="1:7" ht="57.6">
       <c r="A19">
         <v>17</v>
       </c>
@@ -29109,7 +29112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="60">
+    <row r="20" spans="1:7" ht="57.6">
       <c r="A20">
         <v>18</v>
       </c>
@@ -29132,7 +29135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="60">
+    <row r="21" spans="1:7" ht="57.6">
       <c r="A21">
         <v>19</v>
       </c>
@@ -29155,7 +29158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="60">
+    <row r="22" spans="1:7" ht="57.6">
       <c r="A22">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Added new Player class and Globals class. Added code to load the initial pattern from level manager for player's current level stored in playerPrefs.
</commit_message>
<xml_diff>
--- a/Design/Levels.xlsx
+++ b/Design/Levels.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26405"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="_Design Points" sheetId="1" r:id="rId1"/>
     <sheet name="_TASKS" sheetId="2" r:id="rId2"/>
     <sheet name="Levels" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -168,8 +173,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,15 +523,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1"/>
@@ -28588,20 +28593,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -28673,25 +28683,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="11.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="28.8">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="28">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
@@ -28727,7 +28742,7 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="3" spans="1:20" ht="57.6">
+    <row r="3" spans="1:20" ht="56">
       <c r="A3">
         <v>1</v>
       </c>
@@ -28750,7 +28765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="57.6">
+    <row r="4" spans="1:20" ht="56">
       <c r="A4">
         <v>2</v>
       </c>
@@ -28773,7 +28788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="57.6">
+    <row r="5" spans="1:20" ht="56">
       <c r="A5">
         <v>3</v>
       </c>
@@ -28796,7 +28811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="57.6">
+    <row r="6" spans="1:20" ht="56">
       <c r="A6">
         <v>4</v>
       </c>
@@ -28819,7 +28834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="57.6">
+    <row r="7" spans="1:20" ht="56">
       <c r="A7">
         <v>5</v>
       </c>
@@ -28842,7 +28857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="57.6">
+    <row r="8" spans="1:20" ht="56">
       <c r="A8">
         <v>6</v>
       </c>
@@ -28865,7 +28880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="57.6">
+    <row r="9" spans="1:20" ht="56">
       <c r="A9">
         <v>7</v>
       </c>
@@ -28888,7 +28903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="57.6">
+    <row r="10" spans="1:20" ht="56">
       <c r="A10">
         <v>8</v>
       </c>
@@ -28911,7 +28926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="57.6">
+    <row r="11" spans="1:20" ht="56">
       <c r="A11">
         <v>9</v>
       </c>
@@ -28934,7 +28949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="57.6">
+    <row r="12" spans="1:20" ht="56">
       <c r="A12">
         <v>10</v>
       </c>
@@ -28957,7 +28972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="57.6">
+    <row r="13" spans="1:20" ht="56">
       <c r="A13">
         <v>11</v>
       </c>
@@ -28980,7 +28995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="57.6">
+    <row r="14" spans="1:20" ht="56">
       <c r="A14">
         <v>12</v>
       </c>
@@ -29003,7 +29018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="57.6">
+    <row r="15" spans="1:20" ht="56">
       <c r="A15">
         <v>13</v>
       </c>
@@ -29026,7 +29041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="57.6">
+    <row r="16" spans="1:20" ht="56">
       <c r="A16">
         <v>14</v>
       </c>
@@ -29049,7 +29064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="57.6">
+    <row r="17" spans="1:7" ht="56">
       <c r="A17">
         <v>15</v>
       </c>
@@ -29072,7 +29087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="57.6">
+    <row r="18" spans="1:7" ht="56">
       <c r="A18">
         <v>16</v>
       </c>
@@ -29095,7 +29110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="57.6">
+    <row r="19" spans="1:7" ht="56">
       <c r="A19">
         <v>17</v>
       </c>
@@ -29118,7 +29133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="57.6">
+    <row r="20" spans="1:7" ht="56">
       <c r="A20">
         <v>18</v>
       </c>
@@ -29141,7 +29156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="57.6">
+    <row r="21" spans="1:7" ht="56">
       <c r="A21">
         <v>19</v>
       </c>
@@ -29164,7 +29179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="57.6">
+    <row r="22" spans="1:7" ht="56">
       <c r="A22">
         <v>20</v>
       </c>
@@ -29189,6 +29204,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added shuffle guide to level blueprints
</commit_message>
<xml_diff>
--- a/Design/Levels.xlsx
+++ b/Design/Levels.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27022"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="_Design Points" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>Level Design</t>
   </si>
@@ -169,12 +169,24 @@
   <si>
     <t>X</t>
   </si>
+  <si>
+    <t>Shuffle Guide</t>
+  </si>
+  <si>
+    <t>Debug Menu with UI for hooking and displaying variables, may be edit</t>
+  </si>
+  <si>
+    <t>Shuffle pattern!?</t>
+  </si>
+  <si>
+    <t>u,u,u,l,l,l,d,d,d,r</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +204,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -214,10 +242,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -230,8 +262,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -28605,10 +28644,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:C17"/>
+  <dimension ref="A2:C21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -28657,6 +28696,9 @@
       </c>
     </row>
     <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
       <c r="C11" t="s">
         <v>33</v>
       </c>
@@ -28676,13 +28718,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="1:3">
       <c r="B17" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -28697,7 +28753,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -28728,7 +28784,9 @@
       <c r="G1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -28764,6 +28822,9 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="1:20" ht="56">
       <c r="A4">
@@ -28787,6 +28848,9 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="56">
       <c r="A5">
@@ -28810,6 +28874,9 @@
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="H5" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="1:20" ht="56">
       <c r="A6">
@@ -28833,6 +28900,9 @@
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="H6" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:20" ht="56">
       <c r="A7">
@@ -28856,6 +28926,9 @@
       <c r="G7">
         <v>1</v>
       </c>
+      <c r="H7" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:20" ht="56">
       <c r="A8">
@@ -28879,6 +28952,9 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="1:20" ht="56">
       <c r="A9">
@@ -28902,6 +28978,9 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="H9" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:20" ht="56">
       <c r="A10">
@@ -28925,6 +29004,9 @@
       <c r="G10">
         <v>1</v>
       </c>
+      <c r="H10" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:20" ht="56">
       <c r="A11">
@@ -28948,6 +29030,9 @@
       <c r="G11">
         <v>1</v>
       </c>
+      <c r="H11" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:20" ht="56">
       <c r="A12">
@@ -28971,6 +29056,9 @@
       <c r="G12">
         <v>1</v>
       </c>
+      <c r="H12" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:20" ht="56">
       <c r="A13">
@@ -28994,6 +29082,9 @@
       <c r="G13">
         <v>1</v>
       </c>
+      <c r="H13" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="1:20" ht="56">
       <c r="A14">
@@ -29017,6 +29108,9 @@
       <c r="G14">
         <v>1</v>
       </c>
+      <c r="H14" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:20" ht="56">
       <c r="A15">
@@ -29040,6 +29134,9 @@
       <c r="G15">
         <v>1</v>
       </c>
+      <c r="H15" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:20" ht="56">
       <c r="A16">
@@ -29063,8 +29160,11 @@
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="56">
+      <c r="H16" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="56">
       <c r="A17">
         <v>15</v>
       </c>
@@ -29086,8 +29186,11 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="56">
+      <c r="H17" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="56">
       <c r="A18">
         <v>16</v>
       </c>
@@ -29109,8 +29212,11 @@
       <c r="G18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="56">
+      <c r="H18" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="56">
       <c r="A19">
         <v>17</v>
       </c>
@@ -29132,8 +29238,11 @@
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="56">
+      <c r="H19" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="56">
       <c r="A20">
         <v>18</v>
       </c>
@@ -29155,8 +29264,11 @@
       <c r="G20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="56">
+      <c r="H20" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="56">
       <c r="A21">
         <v>19</v>
       </c>
@@ -29178,8 +29290,11 @@
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="56">
+      <c r="H21" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="56">
       <c r="A22">
         <v>20</v>
       </c>
@@ -29201,6 +29316,9 @@
       <c r="G22">
         <v>1</v>
       </c>
+      <c r="H22" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>